<commit_message>
updated from rpiCar and also updated pinout for MPU 6050
</commit_message>
<xml_diff>
--- a/src/PinOuts.xlsx
+++ b/src/PinOuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\rpi_ros_car\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6204627A-F863-4897-8D3E-F84E064462FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A73965-CB17-46AD-BF45-3DE9D9EB7748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21810" yWindow="1185" windowWidth="14790" windowHeight="18840" xr2:uid="{2FED36A7-FEF5-41E5-9472-13578DF8810F}"/>
+    <workbookView xWindow="1770" yWindow="735" windowWidth="17055" windowHeight="19110" xr2:uid="{2FED36A7-FEF5-41E5-9472-13578DF8810F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Raspberry Pi Pinout</t>
   </si>
@@ -147,6 +147,24 @@
   </si>
   <si>
     <t>Grey</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Cooling</t>
+  </si>
+  <si>
+    <t>SCL - MPU 6050</t>
+  </si>
+  <si>
+    <t>SDA - MPU 6050</t>
+  </si>
+  <si>
+    <t>Vcc MPU 6050</t>
+  </si>
+  <si>
+    <t>MPU 6050</t>
   </si>
 </sst>
 </file>
@@ -309,6 +327,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466768</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{071F0F6B-0373-44F5-B88D-883E3E9F2087}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886743" y="342899"/>
+          <a:ext cx="5301572" cy="7934325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,7 +684,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,8 +727,12 @@
         <v>1</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -681,9 +758,14 @@
       <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
@@ -701,9 +783,14 @@
       <c r="C9" s="12">
         <v>3</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="15">
@@ -753,7 +840,9 @@
         <v>9</v>
       </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
     </row>
@@ -874,9 +963,14 @@
         <v>17</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="5"/>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
@@ -1183,10 +1277,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003040CAB79947B945892C065E7D19D555" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="558d1c3654f69919a925c2efc34ef42e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="17184457-8ade-4293-a259-678cc16d8b08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd769d960f2d6c2da010d065c3253806" ns3:_="">
     <xsd:import namespace="17184457-8ade-4293-a259-678cc16d8b08"/>
@@ -1332,22 +1442,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79F2F8C7-7120-467D-B33C-F85C8603F77F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="17184457-8ade-4293-a259-678cc16d8b08"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E16D16-C89A-4648-8352-5CF39F0DD9A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{113042FC-C375-485E-91F7-E39FE03BB93C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1363,28 +1482,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E16D16-C89A-4648-8352-5CF39F0DD9A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79F2F8C7-7120-467D-B33C-F85C8603F77F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="17184457-8ade-4293-a259-678cc16d8b08"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>